<commit_message>
housecleaning + init step 6 cifar10 fig
</commit_message>
<xml_diff>
--- a/projects/1-CNN/results/results-cifar10.xlsx
+++ b/projects/1-CNN/results/results-cifar10.xlsx
@@ -1,43 +1,84 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\Documents\GitHub\neuralnets\projects\1-CNN\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8794A6-3B10-46EE-AE95-429D8DC7DB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>Tilt</t>
+  </si>
+  <si>
+    <t>Contrast</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -46,114 +87,47 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -441,153 +415,141 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Tilt</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Contrast</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Accuracy</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Confidence</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>1.0833</v>
-      </c>
-      <c r="B2" s="1" t="n">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1.0832999999999999</v>
+      </c>
+      <c r="B2" s="1">
         <v>0.3</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.5277500000000001</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.505718186840415</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n">
+      <c r="C2" s="3">
+        <v>0.52775000000000005</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.50571818684041503</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1">
         <v>0.45</v>
       </c>
-      <c r="C3" t="n">
-        <v>0.60275</v>
-      </c>
-      <c r="D3" t="n">
+      <c r="C3" s="3">
+        <v>0.60275000000000001</v>
+      </c>
+      <c r="D3" s="3">
         <v>0.4968130931593478</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.7755</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.610159743335098</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>2.3958</v>
-      </c>
-      <c r="B5" s="1" t="n">
+      <c r="C4">
+        <v>0.77549999999999997</v>
+      </c>
+      <c r="D4">
+        <v>0.61015974333509804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2.3957999999999999</v>
+      </c>
+      <c r="B5" s="1">
         <v>0.3</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>0.59575</v>
       </c>
-      <c r="D5" t="n">
-        <v>0.5305765383914113</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n"/>
-      <c r="B6" s="1" t="n">
+      <c r="D5">
+        <v>0.53057653839141128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1">
         <v>0.45</v>
       </c>
-      <c r="C6" t="n">
-        <v>0.6909999999999999</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.5574910255335271</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n">
+      <c r="C6">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="D6">
+        <v>0.55749102553352714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>0.95875</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1.006004343997687</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="C7">
+        <v>0.95874999999999999</v>
+      </c>
+      <c r="D7">
+        <v>1.0060043439976869</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>0.3</v>
       </c>
-      <c r="C8" t="n">
-        <v>0.64075</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.5486546921171248</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n">
+      <c r="C8">
+        <v>0.64075000000000004</v>
+      </c>
+      <c r="D8">
+        <v>0.54865469211712481</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1">
         <v>0.45</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>0.79</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>0.641829442255199</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="n">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>0.998</v>
       </c>
-      <c r="D10" t="n">
-        <v>1.58897930618003</v>
+      <c r="D10">
+        <v>1.5889793061800299</v>
       </c>
     </row>
   </sheetData>
@@ -596,6 +558,6 @@
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A8:A10"/>
   </mergeCells>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>